<commit_message>
Wired the reports together with the data, only thing remaining is the charts and the styling of the report. After this, need to export each report to a pdf and loop through.
</commit_message>
<xml_diff>
--- a/Input File/Input.xlsx
+++ b/Input File/Input.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="228">
   <si>
     <t>MPConstituency</t>
   </si>
@@ -618,9 +618,6 @@
     <t>Total constituency Population</t>
   </si>
   <si>
-    <t xml:space="preserve">% Population Data available for </t>
-  </si>
-  <si>
     <t xml:space="preserve">%Rural Population </t>
   </si>
   <si>
@@ -636,21 +633,9 @@
     <t>Bengaluru South</t>
   </si>
   <si>
-    <t>Norms for CHCs</t>
-  </si>
-  <si>
-    <t>Norms for PHCs</t>
-  </si>
-  <si>
-    <t>Norms for SCs</t>
-  </si>
-  <si>
     <t>Population</t>
   </si>
   <si>
-    <t>Norms for Beds</t>
-  </si>
-  <si>
     <t>Numberof beds in CHCs</t>
   </si>
   <si>
@@ -702,10 +687,22 @@
     <t>No of Nurses working</t>
   </si>
   <si>
-    <t>AState Avg</t>
-  </si>
-  <si>
     <t>Norm Parameter</t>
+  </si>
+  <si>
+    <t>Norms for No of Sub Centres</t>
+  </si>
+  <si>
+    <t>Norms for No of Primary Health Centers</t>
+  </si>
+  <si>
+    <t>Norms for No of Community Health Centers</t>
+  </si>
+  <si>
+    <t>Norms for No of Beds</t>
+  </si>
+  <si>
+    <t>% Population Data available for</t>
   </si>
 </sst>
 </file>
@@ -1134,7 +1131,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1166,49 +1165,49 @@
         <v>198</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>200</v>
-      </c>
       <c r="G1" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>207</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="P1" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="S1" s="10" t="s">
         <v>221</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>226</v>
       </c>
       <c r="T1" s="10" t="s">
         <v>6</v>
@@ -1231,10 +1230,10 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="G2" s="5"/>
       <c r="Q2" s="6">
@@ -1646,7 +1645,7 @@
         <v>239708</v>
       </c>
       <c r="E8" s="7">
-        <v>0.47426035009261269</v>
+        <v>0.47426035009261303</v>
       </c>
       <c r="F8" s="7">
         <v>0.87126837652477185</v>
@@ -2481,7 +2480,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>24</v>
@@ -2558,10 +2557,10 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>203</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>204</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>23</v>
@@ -2635,7 +2634,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>25</v>
@@ -2712,7 +2711,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>26</v>
@@ -2789,7 +2788,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>28</v>
@@ -2866,7 +2865,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>29</v>
@@ -13425,7 +13424,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:N22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13436,10 +13437,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -13468,7 +13469,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5" s="2">
         <v>35</v>
@@ -13500,7 +13501,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B9" s="4">
         <v>120000</v>
@@ -13508,7 +13509,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B10" s="2">
         <v>30</v>
@@ -13516,7 +13517,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B11" s="2">
         <v>4</v>
@@ -13524,7 +13525,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B12" s="2">
         <v>4</v>
@@ -13532,7 +13533,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B13" s="2">
         <v>1</v>
@@ -13540,7 +13541,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B14" s="2">
         <v>7</v>
@@ -13548,7 +13549,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B15" s="2">
         <v>1</v>
@@ -13556,7 +13557,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Made changes to layout to make it fluid
</commit_message>
<xml_diff>
--- a/Input File/Input.xlsx
+++ b/Input File/Input.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="231">
   <si>
     <t>MPConstituency</t>
   </si>
@@ -703,6 +703,15 @@
   </si>
   <si>
     <t>% Population Data available for</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>This is a test comment</t>
+  </si>
+  <si>
+    <t>This is another test comment</t>
   </si>
 </sst>
 </file>
@@ -1129,11 +1138,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y160"/>
+  <dimension ref="A1:Z160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1151,7 +1158,7 @@
     <col min="23" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" s="11" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1227,8 +1234,11 @@
       <c r="Y1" s="10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z1" s="11" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>214</v>
       </c>
@@ -1246,7 +1256,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
@@ -1322,8 +1332,11 @@
       <c r="Y3" s="6">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z3" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -1399,8 +1412,11 @@
       <c r="Y4" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="Z4" s="6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -1477,7 +1493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1554,7 +1570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>15</v>
       </c>
@@ -1631,7 +1647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
@@ -1708,7 +1724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
@@ -1785,7 +1801,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>30</v>
       </c>
@@ -1862,7 +1878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>30</v>
       </c>
@@ -1939,7 +1955,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
         <v>30</v>
       </c>
@@ -2016,7 +2032,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
         <v>30</v>
       </c>
@@ -2093,7 +2109,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
         <v>37</v>
       </c>
@@ -2170,7 +2186,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
@@ -2247,7 +2263,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
         <v>37</v>
       </c>

</xml_diff>